<commit_message>
Asignación autores recursos en greco mat 7 tema 6
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion06/Escaleta_MA_07_06_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion06/Escaleta_MA_07_06_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion06\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="6975"/>
   </bookViews>
@@ -13,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$P$1:$P$172</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="281">
   <si>
     <t>Asignatura</t>
   </si>
@@ -847,6 +852,21 @@
   </si>
   <si>
     <t>RF_01_02_CO</t>
+  </si>
+  <si>
+    <t>Sandra Ortiz</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
+  </si>
+  <si>
+    <t>Camilo Fuentes</t>
+  </si>
+  <si>
+    <t>Andrés Goméz</t>
   </si>
 </sst>
 </file>
@@ -919,7 +939,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1001,6 +1021,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1223,7 +1267,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1342,18 +1386,36 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1396,24 +1458,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="98">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1571,7 +1622,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1606,7 +1657,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1815,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U172"/>
+  <dimension ref="A1:W172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34:U34"/>
+    <sheetView tabSelected="1" topLeftCell="J11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1837,107 +1888,108 @@
     <col min="12" max="12" width="14.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" style="18" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" style="18" customWidth="1"/>
-    <col min="15" max="15" width="74.42578125" style="18" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="24" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="24" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.7109375" style="24" customWidth="1"/>
-    <col min="21" max="21" width="15" style="24" customWidth="1"/>
-    <col min="22" max="16384" width="11.42578125" style="18"/>
+    <col min="15" max="15" width="74.42578125" style="18" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" style="24" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="24" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" style="24" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="24" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" style="24" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="24" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" style="18" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="60" t="s">
         <v>234</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="58" t="s">
         <v>235</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="66" t="s">
         <v>251</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="52" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="Q1" s="68" t="s">
+      <c r="Q1" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="68" t="s">
+      <c r="S1" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="70" t="s">
+      <c r="T1" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="68" t="s">
+      <c r="U1" s="52" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="59"/>
+    <row r="2" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="63"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="65"/>
       <c r="M2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="69"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="53"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1995,8 +2047,14 @@
       <c r="U3" s="46" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V3" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="W3" s="74">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -2054,8 +2112,14 @@
       <c r="U4" s="46" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V4" s="77" t="s">
+        <v>280</v>
+      </c>
+      <c r="W4" s="74">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -2111,8 +2175,14 @@
       <c r="U5" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V5" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="W5" s="74">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2168,8 +2238,14 @@
       <c r="U6" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V6" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="W6" s="74">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2302,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2284,8 +2360,14 @@
       <c r="U8" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V8" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="W8" s="74">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2345,8 +2427,14 @@
       <c r="U9" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V9" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W9" s="74">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2406,8 +2494,14 @@
       <c r="U10" s="46" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V10" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W10" s="74">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2463,8 +2557,14 @@
       <c r="U11" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V11" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="W11" s="74">
+        <v>45261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2522,8 +2622,14 @@
       <c r="U12" s="46" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V12" s="79" t="s">
+        <v>279</v>
+      </c>
+      <c r="W12" s="74">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2581,8 +2687,14 @@
       <c r="U13" s="46" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V13" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="W13" s="74">
+        <v>39814</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2638,8 +2750,14 @@
       <c r="U14" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V14" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="W14" s="74">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2695,8 +2813,14 @@
       <c r="U15" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V15" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W15" s="74">
+        <v>47453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -2754,8 +2878,14 @@
       <c r="U16" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V16" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W16" s="74">
+        <v>47453</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -2813,8 +2943,14 @@
       <c r="U17" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V17" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W17" s="74">
+        <v>47453</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2872,8 +3008,14 @@
       <c r="U18" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V18" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="W18" s="74">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -2929,8 +3071,9 @@
       <c r="U19" s="46" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V19" s="80"/>
+    </row>
+    <row r="20" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -2988,8 +3131,14 @@
       <c r="U20" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V20" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="W20" s="74">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3047,8 +3196,14 @@
       <c r="U21" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V21" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W21" s="74">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -3105,7 +3260,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -3162,7 +3317,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -3220,8 +3375,14 @@
       <c r="U24" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V24" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="W24" s="74">
+        <v>47088</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -3279,8 +3440,14 @@
       <c r="U25" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V25" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W25" s="74">
+        <v>39448</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -3338,8 +3505,14 @@
       <c r="U26" s="46" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V26" s="79" t="s">
+        <v>279</v>
+      </c>
+      <c r="W26" s="74">
+        <v>38718</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -3395,8 +3568,14 @@
       <c r="U27" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V27" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="W27" s="74">
+        <v>39083</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -3454,8 +3633,14 @@
       <c r="U28" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V28" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W28" s="74">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -3512,7 +3697,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -3570,8 +3755,14 @@
       <c r="U30" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V30" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="W30" s="74">
+        <v>39448</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -3629,8 +3820,14 @@
       <c r="U31" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V31" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W31" s="74">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -3686,8 +3883,14 @@
       <c r="U32" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V32" s="79" t="s">
+        <v>279</v>
+      </c>
+      <c r="W32" s="74">
+        <v>39448</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -3743,8 +3946,14 @@
       <c r="U33" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V33" s="79" t="s">
+        <v>279</v>
+      </c>
+      <c r="W33" s="74">
+        <v>39448</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -3802,8 +4011,14 @@
       <c r="U34" s="46" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V34" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W34" s="74">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -3861,8 +4076,14 @@
       <c r="U35" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V35" s="77" t="s">
+        <v>280</v>
+      </c>
+      <c r="W35" s="74">
+        <v>47453</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
@@ -3905,7 +4126,7 @@
       <c r="T36" s="36"/>
       <c r="U36" s="35"/>
     </row>
-    <row r="37" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -3961,8 +4182,14 @@
       <c r="U37" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V37" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="W37" s="74">
+        <v>39083</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>8</v>
       </c>
@@ -4017,8 +4244,14 @@
       <c r="U38" s="46" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V38" s="78" t="s">
+        <v>278</v>
+      </c>
+      <c r="W38" s="74">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="39"/>
       <c r="B39" s="39"/>
       <c r="C39" s="39"/>
@@ -4036,7 +4269,7 @@
       <c r="T39" s="43"/>
       <c r="U39" s="42"/>
     </row>
-    <row r="40" spans="1:21" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="39"/>
       <c r="B40" s="39"/>
       <c r="C40" s="39"/>
@@ -4054,7 +4287,7 @@
       <c r="T40" s="43"/>
       <c r="U40" s="42"/>
     </row>
-    <row r="41" spans="1:21" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="39"/>
       <c r="B41" s="39"/>
       <c r="C41" s="39"/>
@@ -4566,12 +4799,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4586,6 +4813,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K38">

</xml_diff>